<commit_message>
adding costsfinishing costs script
</commit_message>
<xml_diff>
--- a/cea/databases/lifecycle/LCA_infrastructure.xlsx
+++ b/cea/databases/lifecycle/LCA_infrastructure.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="458" windowWidth="28800" windowHeight="16260" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="458" windowWidth="28800" windowHeight="16260"/>
   </bookViews>
   <sheets>
     <sheet name="dhw" sheetId="4" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="58">
   <si>
     <t>Description</t>
   </si>
@@ -261,6 +261,9 @@
   </si>
   <si>
     <t>ETH network (district heating 43%, heat pump - water/water 28%, heat pump - waste heat 18%, heat recovery 11%)</t>
+  </si>
+  <si>
+    <t>costs_kWh</t>
   </si>
 </sst>
 </file>
@@ -268,7 +271,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="186" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -346,13 +349,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="186" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -373,19 +376,40 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="186" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="186" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="186" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -735,10 +759,436 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="44.3984375" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.46484375" customWidth="1"/>
+    <col min="4" max="4" width="8.46484375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" style="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="11">
+        <v>0</v>
+      </c>
+      <c r="D2" s="11">
+        <v>0</v>
+      </c>
+      <c r="E2" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3">
+        <f>1.3*1.15</f>
+        <v>1.4949999999999999</v>
+      </c>
+      <c r="D3" s="3">
+        <f>1.15*0.0886</f>
+        <v>0.10188999999999999</v>
+      </c>
+      <c r="E3" s="18">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3">
+        <f>1.68*1.15/0.8</f>
+        <v>2.4149999999999996</v>
+      </c>
+      <c r="D4" s="3">
+        <f>1.15*0.12/0.8</f>
+        <v>0.17249999999999996</v>
+      </c>
+      <c r="E4" s="18">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3">
+        <f>1.22*1.15</f>
+        <v>1.4029999999999998</v>
+      </c>
+      <c r="D5" s="3">
+        <f>1.15*0.0869</f>
+        <v>9.9934999999999996E-2</v>
+      </c>
+      <c r="E5" s="18">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3">
+        <f>2.63*0.9*1.15</f>
+        <v>2.7220499999999999</v>
+      </c>
+      <c r="D6" s="3">
+        <f>1.15*0.0413*0.9</f>
+        <v>4.2745500000000006E-2</v>
+      </c>
+      <c r="E6" s="18">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="13">
+        <f>0.2773328387*1.15</f>
+        <v>0.31893276450499997</v>
+      </c>
+      <c r="D7" s="13">
+        <f>1.15*0.014000495</f>
+        <v>1.6100569249999998E-2</v>
+      </c>
+      <c r="E7" s="18">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="3">
+        <f>0.695*1.15</f>
+        <v>0.7992499999999999</v>
+      </c>
+      <c r="D8" s="3">
+        <f>1.15*0.0164</f>
+        <v>1.8860000000000002E-2</v>
+      </c>
+      <c r="E8" s="18">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="3">
+        <f>1.15*0.241</f>
+        <v>0.27714999999999995</v>
+      </c>
+      <c r="D9" s="3">
+        <f>1.15*0.0112</f>
+        <v>1.2879999999999999E-2</v>
+      </c>
+      <c r="E9" s="18">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="3">
+        <f>electricity!C3*1.15/2.7</f>
+        <v>1.120185185185185</v>
+      </c>
+      <c r="D10" s="3">
+        <f>1.15*electricity!D3/2.7</f>
+        <v>1.759074074074074E-2</v>
+      </c>
+      <c r="E10" s="18">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="3">
+        <f>0.795*1.15</f>
+        <v>0.91425000000000001</v>
+      </c>
+      <c r="D11" s="3">
+        <f>1.15*0.0179</f>
+        <v>2.0584999999999999E-2</v>
+      </c>
+      <c r="E11" s="18">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1.55</v>
+      </c>
+      <c r="D12" s="3">
+        <v>8.6900000000000005E-2</v>
+      </c>
+      <c r="E12" s="18">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1</v>
+      </c>
+      <c r="D13" s="3">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="E13" s="18">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1.68</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.112</v>
+      </c>
+      <c r="E14" s="18">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.64100000000000001</v>
+      </c>
+      <c r="D15" s="3">
+        <v>3.7699999999999997E-2</v>
+      </c>
+      <c r="E15" s="18">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="3">
+        <f>C9*0.8</f>
+        <v>0.22171999999999997</v>
+      </c>
+      <c r="D16" s="3">
+        <f>D9*0.8</f>
+        <v>1.0304000000000001E-2</v>
+      </c>
+      <c r="E16" s="18">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="12">
+        <f>C9*0.3+C5*0.7</f>
+        <v>1.0652449999999998</v>
+      </c>
+      <c r="D17" s="12">
+        <f>D9*0.3+D5*0.7</f>
+        <v>7.3818499999999981E-2</v>
+      </c>
+      <c r="E17" s="18">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="12">
+        <f>C9*0.6+C12*0.4</f>
+        <v>0.78629000000000004</v>
+      </c>
+      <c r="D18" s="12">
+        <f>D9*0.6+D12*0.4</f>
+        <v>4.2488000000000005E-2</v>
+      </c>
+      <c r="E18" s="18">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="12">
+        <f>C9*0.6+C13*0.3+C12*0.1</f>
+        <v>0.62129000000000001</v>
+      </c>
+      <c r="D19" s="12">
+        <f>D9*0.6+D13*0.3+D12*0.1</f>
+        <v>2.3168000000000001E-2</v>
+      </c>
+      <c r="E19" s="18">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="12">
+        <v>1.2761111111111112</v>
+      </c>
+      <c r="D20" s="12">
+        <v>4.6404444444444443E-2</v>
+      </c>
+      <c r="E20" s="18">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="12">
+        <v>5.3699999999999998E-2</v>
+      </c>
+      <c r="D21" s="12">
+        <v>9.3999999999999997E-4</v>
+      </c>
+      <c r="E21" s="18">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="3">
+        <f>(0.43*(C21)+0.28*(electricity!C3/2.96)+0.18*0.954+0.11*0)</f>
+        <v>0.44359478378378375</v>
+      </c>
+      <c r="D22" s="3">
+        <f>(0.43*(D21)+0.28*(electricity!D3/2.96)+0.18*0.0149+0.11*0)</f>
+        <v>6.9929567567567578E-3</v>
+      </c>
+      <c r="E22" s="18">
+        <v>0.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:D22"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -749,7 +1199,7 @@
     <col min="4" max="4" width="8.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -762,12 +1212,15 @@
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E1" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="11">
@@ -776,12 +1229,15 @@
       <c r="D2" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E2" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="3">
@@ -792,12 +1248,15 @@
         <f>1.15*0.0886</f>
         <v>0.10188999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E3" s="18">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="3">
@@ -808,12 +1267,15 @@
         <f>1.15*0.12/0.8</f>
         <v>0.17249999999999996</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E4" s="18">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="3">
@@ -824,12 +1286,15 @@
         <f>1.15*0.0869</f>
         <v>9.9934999999999996E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E5" s="18">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="3">
@@ -840,28 +1305,34 @@
         <f>1.15*0.0413*0.9</f>
         <v>4.2745500000000006E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E6" s="18">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="3">
         <f>0.2773328387*1.15</f>
         <v>0.31893276450499997</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="3">
         <f>1.15*0.014000495</f>
         <v>1.6100569249999998E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E7" s="18">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C8" s="3">
@@ -872,12 +1343,15 @@
         <f>1.15*0.0164</f>
         <v>1.8860000000000002E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E8" s="18">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="3">
@@ -888,12 +1362,15 @@
         <f>1.15*0.0112</f>
         <v>1.2879999999999999E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E9" s="18">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C10" s="3">
@@ -901,15 +1378,19 @@
         <v>1.120185185185185</v>
       </c>
       <c r="D10" s="3">
-        <f>1.15*electricity!D3/2.7</f>
+        <f>electricity!D3*1.15/2.7</f>
         <v>1.759074074074074E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E10" s="22">
+        <f>0.2/4</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C11" s="3">
@@ -920,12 +1401,16 @@
         <f>1.15*0.0179</f>
         <v>2.0584999999999999E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E11" s="22">
+        <f>0.2/4</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C12" s="3">
@@ -934,12 +1419,15 @@
       <c r="D12" s="3">
         <v>8.6900000000000005E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E12" s="23">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C13" s="3">
@@ -948,12 +1436,15 @@
       <c r="D13" s="3">
         <v>2.2499999999999999E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E13" s="18">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C14" s="3">
@@ -962,12 +1453,15 @@
       <c r="D14" s="3">
         <v>0.112</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E14" s="18">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C15" s="3">
@@ -976,12 +1470,15 @@
       <c r="D15" s="3">
         <v>3.7699999999999997E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E15" s="18">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C16" s="3">
@@ -992,84 +1489,102 @@
         <f>D9*0.8</f>
         <v>1.0304000000000001E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E16" s="18">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="3">
         <f>C9*0.3+C5*0.7</f>
         <v>1.0652449999999998</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="3">
         <f>D9*0.3+D5*0.7</f>
         <v>7.3818499999999981E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E17" s="18">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C18" s="3">
         <f>C9*0.6+C12*0.4</f>
         <v>0.78629000000000004</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D18" s="3">
         <f>D9*0.6+D12*0.4</f>
         <v>4.2488000000000005E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E18" s="18">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19" s="3">
         <f>C9*0.6+C13*0.3+C12*0.1</f>
         <v>0.62129000000000001</v>
       </c>
-      <c r="D19" s="12">
+      <c r="D19" s="3">
         <f>D9*0.6+D13*0.3+D12*0.1</f>
         <v>2.3168000000000001E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E19" s="18">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" s="10" t="s">
         <v>51</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C20" s="3">
         <v>1.2761111111111112</v>
       </c>
-      <c r="D20" s="12">
+      <c r="D20" s="3">
         <v>4.6404444444444443E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E20" s="18">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" s="10" t="s">
         <v>52</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="12">
+      <c r="C21" s="3">
         <v>5.3699999999999998E-2</v>
       </c>
-      <c r="D21" s="12">
+      <c r="D21" s="3">
         <v>9.3999999999999997E-4</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E21" s="18">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" s="16" t="s">
         <v>56</v>
       </c>
@@ -1084,364 +1599,8 @@
         <f>(0.43*(D21)+0.28*(electricity!D3/2.96)+0.18*0.0149+0.11*0)</f>
         <v>6.9929567567567578E-3</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="43.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.46484375" customWidth="1"/>
-    <col min="4" max="4" width="8.46484375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="11">
-        <v>0</v>
-      </c>
-      <c r="D2" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="3">
-        <f>1.3*1.15</f>
-        <v>1.4949999999999999</v>
-      </c>
-      <c r="D3" s="3">
-        <f>1.15*0.0886</f>
-        <v>0.10188999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="3">
-        <f>1.68*1.15/0.8</f>
-        <v>2.4149999999999996</v>
-      </c>
-      <c r="D4" s="3">
-        <f>1.15*0.12/0.8</f>
-        <v>0.17249999999999996</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="3">
-        <f>1.22*1.15</f>
-        <v>1.4029999999999998</v>
-      </c>
-      <c r="D5" s="3">
-        <f>1.15*0.0869</f>
-        <v>9.9934999999999996E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="3">
-        <f>2.63*0.9*1.15</f>
-        <v>2.7220499999999999</v>
-      </c>
-      <c r="D6" s="3">
-        <f>1.15*0.0413*0.9</f>
-        <v>4.2745500000000006E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="3">
-        <f>0.2773328387*1.15</f>
-        <v>0.31893276450499997</v>
-      </c>
-      <c r="D7" s="3">
-        <f>1.15*0.014000495</f>
-        <v>1.6100569249999998E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="3">
-        <f>0.695*1.15</f>
-        <v>0.7992499999999999</v>
-      </c>
-      <c r="D8" s="3">
-        <f>1.15*0.0164</f>
-        <v>1.8860000000000002E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="3">
-        <f>1.15*0.241</f>
-        <v>0.27714999999999995</v>
-      </c>
-      <c r="D9" s="3">
-        <f>1.15*0.0112</f>
-        <v>1.2879999999999999E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="3">
-        <f>electricity!C3*1.15/2.7</f>
-        <v>1.120185185185185</v>
-      </c>
-      <c r="D10" s="3">
-        <f>electricity!D3*1.15/2.7</f>
-        <v>1.759074074074074E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="3">
-        <f>0.795*1.15</f>
-        <v>0.91425000000000001</v>
-      </c>
-      <c r="D11" s="3">
-        <f>1.15*0.0179</f>
-        <v>2.0584999999999999E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="3">
-        <v>1.55</v>
-      </c>
-      <c r="D12" s="3">
-        <v>8.6900000000000005E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A13" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="3">
-        <v>1</v>
-      </c>
-      <c r="D13" s="3">
-        <v>2.2499999999999999E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="3">
-        <v>1.68</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0.112</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A15" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="3">
-        <v>0.64100000000000001</v>
-      </c>
-      <c r="D15" s="3">
-        <v>3.7699999999999997E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A16" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="3">
-        <f>C9*0.8</f>
-        <v>0.22171999999999997</v>
-      </c>
-      <c r="D16" s="3">
-        <f>D9*0.8</f>
-        <v>1.0304000000000001E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="3">
-        <f>C9*0.3+C5*0.7</f>
-        <v>1.0652449999999998</v>
-      </c>
-      <c r="D17" s="3">
-        <f>D9*0.3+D5*0.7</f>
-        <v>7.3818499999999981E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="3">
-        <f>C9*0.6+C12*0.4</f>
-        <v>0.78629000000000004</v>
-      </c>
-      <c r="D18" s="3">
-        <f>D9*0.6+D12*0.4</f>
-        <v>4.2488000000000005E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="3">
-        <f>C9*0.6+C13*0.3+C12*0.1</f>
-        <v>0.62129000000000001</v>
-      </c>
-      <c r="D19" s="3">
-        <f>D9*0.6+D13*0.3+D12*0.1</f>
-        <v>2.3168000000000001E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A20" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="3">
-        <v>1.2761111111111112</v>
-      </c>
-      <c r="D20" s="3">
-        <v>4.6404444444444443E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A21" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="3">
-        <v>5.3699999999999998E-2</v>
-      </c>
-      <c r="D21" s="3">
-        <v>9.3999999999999997E-4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A22" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="3">
-        <f>(0.43*(C21)+0.28*(electricity!C3/2.96)+0.18*0.954+0.11*0)</f>
-        <v>0.44359478378378375</v>
-      </c>
-      <c r="D22" s="3">
-        <f>(0.43*(D21)+0.28*(electricity!D3/2.96)+0.18*0.0149+0.11*0)</f>
-        <v>6.9929567567567578E-3</v>
+      <c r="E22" s="18">
+        <v>0.08</v>
       </c>
     </row>
   </sheetData>
@@ -1453,10 +1612,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1467,7 +1626,7 @@
     <col min="4" max="4" width="6.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1480,8 +1639,11 @@
       <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E1" s="19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1494,8 +1656,11 @@
       <c r="D2" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E2" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
@@ -1508,8 +1673,12 @@
       <c r="D3" s="14">
         <v>1.8860000000000002E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E3" s="21">
+        <f>0.2/2.7</f>
+        <v>7.407407407407407E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
@@ -1522,8 +1691,12 @@
       <c r="D4" s="14">
         <v>1.759074074074074E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E4" s="21">
+        <f t="shared" ref="E4:E6" si="0">0.2/2.7</f>
+        <v>7.407407407407407E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
@@ -1538,8 +1711,12 @@
         <f>D6*0.8</f>
         <v>1.956260204185213E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E5" s="21">
+        <f t="shared" si="0"/>
+        <v>7.407407407407407E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>53</v>
       </c>
@@ -1551,6 +1728,10 @@
       </c>
       <c r="D6" s="14">
         <v>2.4453252552315164E-3</v>
+      </c>
+      <c r="E6" s="21">
+        <f t="shared" si="0"/>
+        <v>7.407407407407407E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1561,18 +1742,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1585,8 +1766,11 @@
       <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E1" s="19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
@@ -1599,8 +1783,11 @@
       <c r="D2" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E2" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="8" t="s">
         <v>46</v>
       </c>
@@ -1613,8 +1800,11 @@
       <c r="D3" s="14">
         <v>4.1300000000000003E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E3" s="21">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="8" t="s">
         <v>43</v>
       </c>
@@ -1627,8 +1817,11 @@
       <c r="D4" s="14">
         <v>2.0199999999999999E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E4" s="18">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
@@ -1641,8 +1834,11 @@
       <c r="D5" s="14">
         <v>1.0800000000000001E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E5" s="18">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="8" t="s">
         <v>44</v>
       </c>
@@ -1657,8 +1853,11 @@
         <f>D4*0.3+D3*0.7</f>
         <v>3.4970000000000001E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E6" s="21">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="8" t="s">
         <v>45</v>
       </c>
@@ -1672,6 +1871,9 @@
       <c r="D7" s="14">
         <f>D5*0.3+D3*0.7</f>
         <v>3.2150000000000005E-2</v>
+      </c>
+      <c r="E7" s="21">
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes to dhw in database
</commit_message>
<xml_diff>
--- a/cea/databases/lifecycle/LCA_infrastructure.xlsx
+++ b/cea/databases/lifecycle/LCA_infrastructure.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jimeno\Documents\CEAforArcGIS\cea\databases\lifecycle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bhargava\Documents\GitHub\CEAforArcGIS\cea\databases\lifecycle\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="458" windowWidth="28800" windowHeight="16260"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260"/>
   </bookViews>
   <sheets>
     <sheet name="dhw" sheetId="4" r:id="rId1"/>
@@ -762,19 +762,19 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="44.3984375" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.46484375" customWidth="1"/>
-    <col min="4" max="4" width="8.46484375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.36328125" customWidth="1"/>
+    <col min="2" max="2" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.453125" customWidth="1"/>
+    <col min="4" max="4" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6328125" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -791,7 +791,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -808,7 +808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -827,7 +827,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -846,7 +846,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -865,7 +865,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -884,7 +884,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -903,7 +903,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -922,7 +922,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -938,10 +938,10 @@
         <v>1.2879999999999999E-2</v>
       </c>
       <c r="E9" s="18">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>55</v>
       </c>
@@ -956,11 +956,12 @@
         <f>1.15*electricity!D3/2.7</f>
         <v>1.759074074074074E-2</v>
       </c>
-      <c r="E10" s="18">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E10" s="22">
+        <f>0.2/4</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -975,11 +976,12 @@
         <f>1.15*0.0179</f>
         <v>2.0584999999999999E-2</v>
       </c>
-      <c r="E11" s="18">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E11" s="22">
+        <f>0.2/4</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
@@ -992,11 +994,11 @@
       <c r="D12" s="3">
         <v>8.6900000000000005E-2</v>
       </c>
-      <c r="E12" s="18">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E12" s="23">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>47</v>
       </c>
@@ -1010,10 +1012,10 @@
         <v>2.2499999999999999E-2</v>
       </c>
       <c r="E13" s="18">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>48</v>
       </c>
@@ -1027,10 +1029,10 @@
         <v>0.112</v>
       </c>
       <c r="E14" s="18">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>49</v>
       </c>
@@ -1044,10 +1046,10 @@
         <v>3.7699999999999997E-2</v>
       </c>
       <c r="E15" s="18">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>50</v>
       </c>
@@ -1063,10 +1065,10 @@
         <v>1.0304000000000001E-2</v>
       </c>
       <c r="E16" s="18">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -1082,10 +1084,10 @@
         <v>7.3818499999999981E-2</v>
       </c>
       <c r="E17" s="18">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
@@ -1101,10 +1103,10 @@
         <v>4.2488000000000005E-2</v>
       </c>
       <c r="E18" s="18">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
@@ -1120,10 +1122,10 @@
         <v>2.3168000000000001E-2</v>
       </c>
       <c r="E19" s="18">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
         <v>51</v>
       </c>
@@ -1137,10 +1139,10 @@
         <v>4.6404444444444443E-2</v>
       </c>
       <c r="E20" s="18">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
         <v>52</v>
       </c>
@@ -1154,10 +1156,10 @@
         <v>9.3999999999999997E-4</v>
       </c>
       <c r="E21" s="18">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="16" t="s">
         <v>56</v>
       </c>
@@ -1173,7 +1175,7 @@
         <v>6.9929567567567578E-3</v>
       </c>
       <c r="E22" s="18">
-        <v>0.2</v>
+        <v>0.08</v>
       </c>
     </row>
   </sheetData>
@@ -1188,18 +1190,18 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E2" sqref="E2:E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="43.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.46484375" customWidth="1"/>
-    <col min="4" max="4" width="8.46484375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.453125" customWidth="1"/>
+    <col min="4" max="4" width="8.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1216,7 +1218,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -1233,7 +1235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -1252,7 +1254,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -1271,7 +1273,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -1290,7 +1292,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -1309,7 +1311,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -1328,7 +1330,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -1347,7 +1349,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -1366,7 +1368,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -1386,7 +1388,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -1406,7 +1408,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
@@ -1423,7 +1425,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>47</v>
       </c>
@@ -1440,7 +1442,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>48</v>
       </c>
@@ -1457,7 +1459,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>49</v>
       </c>
@@ -1474,7 +1476,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>50</v>
       </c>
@@ -1493,7 +1495,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -1512,7 +1514,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
@@ -1531,7 +1533,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
@@ -1550,7 +1552,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
         <v>51</v>
       </c>
@@ -1567,7 +1569,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
         <v>52</v>
       </c>
@@ -1584,7 +1586,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="16" t="s">
         <v>56</v>
       </c>
@@ -1618,15 +1620,15 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" customWidth="1"/>
+    <col min="1" max="1" width="31.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.36328125" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.46484375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1643,7 +1645,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1660,7 +1662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
@@ -1678,7 +1680,7 @@
         <v>7.407407407407407E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
@@ -1696,7 +1698,7 @@
         <v>7.407407407407407E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
@@ -1716,7 +1718,7 @@
         <v>7.407407407407407E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>53</v>
       </c>
@@ -1748,12 +1750,12 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" customWidth="1"/>
+    <col min="1" max="1" width="35.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1770,7 +1772,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
@@ -1787,7 +1789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>46</v>
       </c>
@@ -1804,7 +1806,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>43</v>
       </c>
@@ -1821,7 +1823,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
@@ -1838,7 +1840,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>44</v>
       </c>
@@ -1857,7 +1859,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
adding emisisons of systems in singapore (roughly estimated)
</commit_message>
<xml_diff>
--- a/cea/databases/lifecycle/LCA_infrastructure.xlsx
+++ b/cea/databases/lifecycle/LCA_infrastructure.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bhargava\Documents\GitHub\CEAforArcGIS\cea\databases\lifecycle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jimeno\Documents\CityEnergyAnalyst\cea\databases\lifecycle\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260"/>
+    <workbookView xWindow="0" yWindow="458" windowWidth="28800" windowHeight="16260" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="dhw" sheetId="4" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="60">
   <si>
     <t>Description</t>
   </si>
@@ -264,6 +264,12 @@
   </si>
   <si>
     <t>costs_kWh</t>
+  </si>
+  <si>
+    <t>Singaporean consumer mix</t>
+  </si>
+  <si>
+    <t>district cooling network - air-air</t>
   </si>
 </sst>
 </file>
@@ -321,7 +327,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -344,12 +350,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -409,6 +426,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -761,20 +787,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="44.36328125" customWidth="1"/>
-    <col min="2" max="2" width="6.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.453125" customWidth="1"/>
-    <col min="4" max="4" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.6328125" style="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.33203125" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.46484375" customWidth="1"/>
+    <col min="4" max="4" width="8.46484375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.59765625" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -791,7 +817,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -808,7 +834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -827,7 +853,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -846,7 +872,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -865,7 +891,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -884,7 +910,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -903,7 +929,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -922,7 +948,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -941,7 +967,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>55</v>
       </c>
@@ -961,7 +987,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -981,7 +1007,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
@@ -998,7 +1024,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>47</v>
       </c>
@@ -1015,7 +1041,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>48</v>
       </c>
@@ -1032,7 +1058,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>49</v>
       </c>
@@ -1049,7 +1075,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>50</v>
       </c>
@@ -1068,7 +1094,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -1087,7 +1113,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
@@ -1106,7 +1132,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
@@ -1125,7 +1151,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" s="10" t="s">
         <v>51</v>
       </c>
@@ -1142,7 +1168,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" s="10" t="s">
         <v>52</v>
       </c>
@@ -1159,7 +1185,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" s="16" t="s">
         <v>56</v>
       </c>
@@ -1190,18 +1216,18 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E22"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="43.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.453125" customWidth="1"/>
-    <col min="4" max="4" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.06640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.46484375" customWidth="1"/>
+    <col min="4" max="4" width="8.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1218,7 +1244,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -1235,7 +1261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -1254,7 +1280,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -1273,7 +1299,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -1292,7 +1318,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -1311,7 +1337,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -1330,7 +1356,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -1349,7 +1375,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -1368,7 +1394,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -1388,7 +1414,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -1408,7 +1434,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
@@ -1425,7 +1451,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>47</v>
       </c>
@@ -1442,7 +1468,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>48</v>
       </c>
@@ -1459,7 +1485,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>49</v>
       </c>
@@ -1476,7 +1502,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>50</v>
       </c>
@@ -1495,7 +1521,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -1514,7 +1540,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
@@ -1533,7 +1559,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
@@ -1552,7 +1578,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" s="10" t="s">
         <v>51</v>
       </c>
@@ -1569,7 +1595,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" s="10" t="s">
         <v>52</v>
       </c>
@@ -1586,7 +1612,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" s="16" t="s">
         <v>56</v>
       </c>
@@ -1614,21 +1640,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="31.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.36328125" customWidth="1"/>
+    <col min="1" max="1" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1645,7 +1671,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1662,7 +1688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
@@ -1680,7 +1706,7 @@
         <v>7.407407407407407E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
@@ -1694,11 +1720,11 @@
         <v>1.759074074074074E-2</v>
       </c>
       <c r="E4" s="21">
-        <f t="shared" ref="E4:E6" si="0">0.2/2.7</f>
+        <f t="shared" ref="E4:E7" si="0">0.2/2.7</f>
         <v>7.407407407407407E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
@@ -1718,7 +1744,7 @@
         <v>7.407407407407407E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>53</v>
       </c>
@@ -1735,6 +1761,29 @@
         <f t="shared" si="0"/>
         <v>7.407407407407407E-2</v>
       </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="14">
+        <f>electricity!C8/4</f>
+        <v>0.87687499999999985</v>
+      </c>
+      <c r="D7" s="14">
+        <f>electricity!D8/4</f>
+        <v>6.2459374999999998E-2</v>
+      </c>
+      <c r="E7" s="14">
+        <f>electricity!E8/4</f>
+        <v>6.7500000000000004E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.3" footer="0.3"/>
@@ -1744,18 +1793,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="35.6328125" customWidth="1"/>
+    <col min="1" max="1" width="35.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1772,7 +1821,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
@@ -1789,7 +1838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="8" t="s">
         <v>46</v>
       </c>
@@ -1806,7 +1855,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="8" t="s">
         <v>43</v>
       </c>
@@ -1819,11 +1868,11 @@
       <c r="D4" s="14">
         <v>2.0199999999999999E-2</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="24">
         <v>0.6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
@@ -1836,11 +1885,11 @@
       <c r="D5" s="14">
         <v>1.0800000000000001E-2</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="24">
         <v>0.7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="8" t="s">
         <v>44</v>
       </c>
@@ -1859,7 +1908,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="8" t="s">
         <v>45</v>
       </c>
@@ -1876,6 +1925,25 @@
       </c>
       <c r="E7" s="21">
         <v>0.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="21">
+        <f>heating!C5/0.4</f>
+        <v>3.5074999999999994</v>
+      </c>
+      <c r="D8" s="21">
+        <f>heating!D5/0.4</f>
+        <v>0.24983749999999999</v>
+      </c>
+      <c r="E8" s="21">
+        <v>0.27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>